<commit_message>
workshop documentation and typo fix
</commit_message>
<xml_diff>
--- a/Samples/Templates/Leases.xlsx
+++ b/Samples/Templates/Leases.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10908"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10916"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6BD5683-31AC-DF46-A07A-384BB74837BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B577385E-87D6-0E4F-8E10-9A46611DDF09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="26160" yWindow="500" windowWidth="25040" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10780" yWindow="500" windowWidth="40420" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Leases" sheetId="1" r:id="rId1"/>
@@ -56,9 +56,6 @@
     <t>Dual Residential Pod</t>
   </si>
   <si>
-    <t>Tripple Residential Pod</t>
-  </si>
-  <si>
     <t>Two private and spacious bedrooms, each equipped with a temperature-regulating system, offering breathtaking views of the lunar landscape through reinforced transparent panels. Bedrooms are fitted with built-in storage for personal items and lunar suits.</t>
   </si>
   <si>
@@ -540,6 +537,9 @@
   </si>
   <si>
     <t>BedRooms</t>
+  </si>
+  <si>
+    <t>Triple Residential Pod</t>
   </si>
 </sst>
 </file>
@@ -995,7 +995,7 @@
   <dimension ref="B10:K60"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A6" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1019,25 +1019,25 @@
         <v>1</v>
       </c>
       <c r="D10" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E10" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F10" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G10" t="s">
         <v>2</v>
       </c>
       <c r="H10" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="I10" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="J10" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="K10" t="s">
         <v>5</v>
@@ -1045,10 +1045,10 @@
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C11" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D11" s="2">
         <v>45374</v>
@@ -1060,7 +1060,7 @@
         <v>46477</v>
       </c>
       <c r="G11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H11" t="str">
         <f>VLOOKUP($G11,Properties[],2,FALSE)</f>
@@ -1081,10 +1081,10 @@
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C12" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D12" s="2">
         <v>45363</v>
@@ -1096,7 +1096,7 @@
         <v>46477</v>
       </c>
       <c r="G12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H12" t="str">
         <f>VLOOKUP($G12,Properties[],2,FALSE)</f>
@@ -1117,10 +1117,10 @@
     </row>
     <row r="13" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C13" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D13" s="2">
         <v>45418</v>
@@ -1132,7 +1132,7 @@
         <v>46538</v>
       </c>
       <c r="G13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H13" t="str">
         <f>VLOOKUP($G13,Properties[],2,FALSE)</f>
@@ -1153,10 +1153,10 @@
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C14" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D14" s="2">
         <v>45418</v>
@@ -1168,7 +1168,7 @@
         <v>46538</v>
       </c>
       <c r="G14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H14" t="str">
         <f>VLOOKUP($G14,Properties[],2,FALSE)</f>
@@ -1189,10 +1189,10 @@
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C15" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D15" s="2">
         <v>45498</v>
@@ -1204,7 +1204,7 @@
         <v>46599</v>
       </c>
       <c r="G15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H15" t="str">
         <f>VLOOKUP($G15,Properties[],2,FALSE)</f>
@@ -1225,10 +1225,10 @@
     </row>
     <row r="16" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C16" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D16" s="2">
         <v>45379</v>
@@ -1240,7 +1240,7 @@
         <v>46477</v>
       </c>
       <c r="G16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H16" t="str">
         <f>VLOOKUP($G16,Properties[],2,FALSE)</f>
@@ -1261,10 +1261,10 @@
     </row>
     <row r="17" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C17" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D17" s="2">
         <v>45486</v>
@@ -1276,7 +1276,7 @@
         <v>46599</v>
       </c>
       <c r="G17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H17" t="str">
         <f>VLOOKUP($G17,Properties[],2,FALSE)</f>
@@ -1297,10 +1297,10 @@
     </row>
     <row r="18" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C18" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D18" s="2">
         <v>45407</v>
@@ -1312,7 +1312,7 @@
         <v>46507</v>
       </c>
       <c r="G18" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H18" t="str">
         <f>VLOOKUP($G18,Properties[],2,FALSE)</f>
@@ -1333,10 +1333,10 @@
     </row>
     <row r="19" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C19" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D19" s="2">
         <v>45360</v>
@@ -1348,7 +1348,7 @@
         <v>46477</v>
       </c>
       <c r="G19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H19" t="str">
         <f>VLOOKUP($G19,Properties[],2,FALSE)</f>
@@ -1369,10 +1369,10 @@
     </row>
     <row r="20" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C20" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D20" s="2">
         <v>45421</v>
@@ -1384,7 +1384,7 @@
         <v>46538</v>
       </c>
       <c r="G20" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H20" t="str">
         <f>VLOOKUP($G20,Properties[],2,FALSE)</f>
@@ -1405,10 +1405,10 @@
     </row>
     <row r="21" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C21" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D21" s="2">
         <v>45409</v>
@@ -1420,7 +1420,7 @@
         <v>46507</v>
       </c>
       <c r="G21" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H21" t="str">
         <f>VLOOKUP($G21,Properties[],2,FALSE)</f>
@@ -1441,10 +1441,10 @@
     </row>
     <row r="22" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C22" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D22" s="2">
         <v>45371</v>
@@ -1456,7 +1456,7 @@
         <v>46477</v>
       </c>
       <c r="G22" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H22" t="str">
         <f>VLOOKUP($G22,Properties[],2,FALSE)</f>
@@ -1477,10 +1477,10 @@
     </row>
     <row r="23" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C23" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D23" s="2">
         <v>45487</v>
@@ -1492,7 +1492,7 @@
         <v>46599</v>
       </c>
       <c r="G23" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H23" t="str">
         <f>VLOOKUP($G23,Properties[],2,FALSE)</f>
@@ -1513,10 +1513,10 @@
     </row>
     <row r="24" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C24" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D24" s="2">
         <v>45419</v>
@@ -1528,7 +1528,7 @@
         <v>46538</v>
       </c>
       <c r="G24" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H24" t="str">
         <f>VLOOKUP($G24,Properties[],2,FALSE)</f>
@@ -1549,10 +1549,10 @@
     </row>
     <row r="25" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C25" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D25" s="2">
         <v>45396</v>
@@ -1564,7 +1564,7 @@
         <v>46507</v>
       </c>
       <c r="G25" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H25" t="str">
         <f>VLOOKUP($G25,Properties[],2,FALSE)</f>
@@ -1585,10 +1585,10 @@
     </row>
     <row r="26" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C26" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D26" s="2">
         <v>45476</v>
@@ -1600,7 +1600,7 @@
         <v>46599</v>
       </c>
       <c r="G26" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H26" t="str">
         <f>VLOOKUP($G26,Properties[],2,FALSE)</f>
@@ -1621,10 +1621,10 @@
     </row>
     <row r="27" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C27" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D27" s="2">
         <v>45342</v>
@@ -1636,7 +1636,7 @@
         <v>46446</v>
       </c>
       <c r="G27" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H27" t="str">
         <f>VLOOKUP($G27,Properties[],2,FALSE)</f>
@@ -1657,10 +1657,10 @@
     </row>
     <row r="28" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C28" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D28" s="2">
         <v>45353</v>
@@ -1672,7 +1672,7 @@
         <v>46477</v>
       </c>
       <c r="G28" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H28" t="str">
         <f>VLOOKUP($G28,Properties[],2,FALSE)</f>
@@ -1693,10 +1693,10 @@
     </row>
     <row r="29" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C29" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D29" s="2">
         <v>45389</v>
@@ -1708,7 +1708,7 @@
         <v>46507</v>
       </c>
       <c r="G29" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H29" t="str">
         <f>VLOOKUP($G29,Properties[],2,FALSE)</f>
@@ -1729,10 +1729,10 @@
     </row>
     <row r="30" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B30" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C30" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D30" s="2">
         <v>45333</v>
@@ -1744,7 +1744,7 @@
         <v>46446</v>
       </c>
       <c r="G30" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H30" t="str">
         <f>VLOOKUP($G30,Properties[],2,FALSE)</f>
@@ -1765,10 +1765,10 @@
     </row>
     <row r="31" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B31" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C31" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D31" s="2">
         <v>45472</v>
@@ -1780,11 +1780,11 @@
         <v>46568</v>
       </c>
       <c r="G31" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H31" t="str">
         <f>VLOOKUP($G31,Properties[],2,FALSE)</f>
-        <v>Tripple Residential Pod</v>
+        <v>Triple Residential Pod</v>
       </c>
       <c r="I31" t="str">
         <f>VLOOKUP($G31,Properties[],3,FALSE)</f>
@@ -1801,10 +1801,10 @@
     </row>
     <row r="32" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C32" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D32" s="2">
         <v>45431</v>
@@ -1816,11 +1816,11 @@
         <v>46538</v>
       </c>
       <c r="G32" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H32" t="str">
         <f>VLOOKUP($G32,Properties[],2,FALSE)</f>
-        <v>Tripple Residential Pod</v>
+        <v>Triple Residential Pod</v>
       </c>
       <c r="I32" t="str">
         <f>VLOOKUP($G32,Properties[],3,FALSE)</f>
@@ -1837,10 +1837,10 @@
     </row>
     <row r="33" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B33" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C33" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D33" s="2">
         <v>45419</v>
@@ -1852,11 +1852,11 @@
         <v>46538</v>
       </c>
       <c r="G33" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H33" t="str">
         <f>VLOOKUP($G33,Properties[],2,FALSE)</f>
-        <v>Tripple Residential Pod</v>
+        <v>Triple Residential Pod</v>
       </c>
       <c r="I33" t="str">
         <f>VLOOKUP($G33,Properties[],3,FALSE)</f>
@@ -1873,10 +1873,10 @@
     </row>
     <row r="34" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B34" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C34" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D34" s="2">
         <v>45403</v>
@@ -1888,11 +1888,11 @@
         <v>46507</v>
       </c>
       <c r="G34" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H34" t="str">
         <f>VLOOKUP($G34,Properties[],2,FALSE)</f>
-        <v>Tripple Residential Pod</v>
+        <v>Triple Residential Pod</v>
       </c>
       <c r="I34" t="str">
         <f>VLOOKUP($G34,Properties[],3,FALSE)</f>
@@ -1909,10 +1909,10 @@
     </row>
     <row r="35" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B35" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C35" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D35" s="2">
         <v>45395</v>
@@ -1924,11 +1924,11 @@
         <v>46507</v>
       </c>
       <c r="G35" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H35" t="str">
         <f>VLOOKUP($G35,Properties[],2,FALSE)</f>
-        <v>Tripple Residential Pod</v>
+        <v>Triple Residential Pod</v>
       </c>
       <c r="I35" t="str">
         <f>VLOOKUP($G35,Properties[],3,FALSE)</f>
@@ -1945,10 +1945,10 @@
     </row>
     <row r="36" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B36" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C36" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D36" s="2">
         <v>45372</v>
@@ -1960,11 +1960,11 @@
         <v>46477</v>
       </c>
       <c r="G36" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H36" t="str">
         <f>VLOOKUP($G36,Properties[],2,FALSE)</f>
-        <v>Tripple Residential Pod</v>
+        <v>Triple Residential Pod</v>
       </c>
       <c r="I36" t="str">
         <f>VLOOKUP($G36,Properties[],3,FALSE)</f>
@@ -1981,10 +1981,10 @@
     </row>
     <row r="37" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B37" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C37" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D37" s="2">
         <v>45430</v>
@@ -1996,11 +1996,11 @@
         <v>46538</v>
       </c>
       <c r="G37" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H37" t="str">
         <f>VLOOKUP($G37,Properties[],2,FALSE)</f>
-        <v>Tripple Residential Pod</v>
+        <v>Triple Residential Pod</v>
       </c>
       <c r="I37" t="str">
         <f>VLOOKUP($G37,Properties[],3,FALSE)</f>
@@ -2017,10 +2017,10 @@
     </row>
     <row r="38" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B38" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C38" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D38" s="2">
         <v>45433</v>
@@ -2032,11 +2032,11 @@
         <v>46538</v>
       </c>
       <c r="G38" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H38" t="str">
         <f>VLOOKUP($G38,Properties[],2,FALSE)</f>
-        <v>Tripple Residential Pod</v>
+        <v>Triple Residential Pod</v>
       </c>
       <c r="I38" t="str">
         <f>VLOOKUP($G38,Properties[],3,FALSE)</f>
@@ -2053,10 +2053,10 @@
     </row>
     <row r="39" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B39" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C39" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D39" s="2">
         <v>45454</v>
@@ -2068,11 +2068,11 @@
         <v>46568</v>
       </c>
       <c r="G39" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H39" t="str">
         <f>VLOOKUP($G39,Properties[],2,FALSE)</f>
-        <v>Tripple Residential Pod</v>
+        <v>Triple Residential Pod</v>
       </c>
       <c r="I39" t="str">
         <f>VLOOKUP($G39,Properties[],3,FALSE)</f>
@@ -2089,10 +2089,10 @@
     </row>
     <row r="40" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B40" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C40" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D40" s="2">
         <v>45487</v>
@@ -2104,11 +2104,11 @@
         <v>46599</v>
       </c>
       <c r="G40" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H40" t="str">
         <f>VLOOKUP($G40,Properties[],2,FALSE)</f>
-        <v>Tripple Residential Pod</v>
+        <v>Triple Residential Pod</v>
       </c>
       <c r="I40" t="str">
         <f>VLOOKUP($G40,Properties[],3,FALSE)</f>
@@ -2125,10 +2125,10 @@
     </row>
     <row r="41" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B41" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C41" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D41" s="2">
         <v>45406</v>
@@ -2140,7 +2140,7 @@
         <v>46507</v>
       </c>
       <c r="G41" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H41" t="str">
         <f>VLOOKUP($G41,Properties[],2,FALSE)</f>
@@ -2161,10 +2161,10 @@
     </row>
     <row r="42" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B42" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C42" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D42" s="2">
         <v>45412</v>
@@ -2176,7 +2176,7 @@
         <v>46507</v>
       </c>
       <c r="G42" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H42" t="str">
         <f>VLOOKUP($G42,Properties[],2,FALSE)</f>
@@ -2197,10 +2197,10 @@
     </row>
     <row r="43" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B43" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C43" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D43" s="2">
         <v>45334</v>
@@ -2212,7 +2212,7 @@
         <v>46446</v>
       </c>
       <c r="G43" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H43" t="str">
         <f>VLOOKUP($G43,Properties[],2,FALSE)</f>
@@ -2233,10 +2233,10 @@
     </row>
     <row r="44" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B44" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C44" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D44" s="2">
         <v>45331</v>
@@ -2248,7 +2248,7 @@
         <v>46446</v>
       </c>
       <c r="G44" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H44" t="str">
         <f>VLOOKUP($G44,Properties[],2,FALSE)</f>
@@ -2269,10 +2269,10 @@
     </row>
     <row r="45" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B45" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C45" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D45" s="2">
         <v>45407</v>
@@ -2284,7 +2284,7 @@
         <v>46507</v>
       </c>
       <c r="G45" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H45" t="str">
         <f>VLOOKUP($G45,Properties[],2,FALSE)</f>
@@ -2305,10 +2305,10 @@
     </row>
     <row r="46" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B46" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C46" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D46" s="2">
         <v>45326</v>
@@ -2320,7 +2320,7 @@
         <v>46446</v>
       </c>
       <c r="G46" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H46" t="str">
         <f>VLOOKUP($G46,Properties[],2,FALSE)</f>
@@ -2341,10 +2341,10 @@
     </row>
     <row r="47" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B47" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C47" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D47" s="2">
         <v>45345</v>
@@ -2356,7 +2356,7 @@
         <v>46446</v>
       </c>
       <c r="G47" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H47" t="str">
         <f>VLOOKUP($G47,Properties[],2,FALSE)</f>
@@ -2377,10 +2377,10 @@
     </row>
     <row r="48" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B48" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C48" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D48" s="2">
         <v>45328</v>
@@ -2392,7 +2392,7 @@
         <v>46446</v>
       </c>
       <c r="G48" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H48" t="str">
         <f>VLOOKUP($G48,Properties[],2,FALSE)</f>
@@ -2413,10 +2413,10 @@
     </row>
     <row r="49" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B49" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C49" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D49" s="2">
         <v>45400</v>
@@ -2428,7 +2428,7 @@
         <v>46507</v>
       </c>
       <c r="G49" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H49" t="str">
         <f>VLOOKUP($G49,Properties[],2,FALSE)</f>
@@ -2449,10 +2449,10 @@
     </row>
     <row r="50" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B50" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C50" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D50" s="2">
         <v>45364</v>
@@ -2464,7 +2464,7 @@
         <v>46477</v>
       </c>
       <c r="G50" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H50" t="str">
         <f>VLOOKUP($G50,Properties[],2,FALSE)</f>
@@ -2485,10 +2485,10 @@
     </row>
     <row r="51" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B51" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C51" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D51" s="2">
         <v>45434</v>
@@ -2500,7 +2500,7 @@
         <v>46538</v>
       </c>
       <c r="G51" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H51" t="str">
         <f>VLOOKUP($G51,Properties[],2,FALSE)</f>
@@ -2521,10 +2521,10 @@
     </row>
     <row r="52" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B52" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C52" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D52" s="2">
         <v>45331</v>
@@ -2536,7 +2536,7 @@
         <v>46446</v>
       </c>
       <c r="G52" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H52" t="str">
         <f>VLOOKUP($G52,Properties[],2,FALSE)</f>
@@ -2557,10 +2557,10 @@
     </row>
     <row r="53" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B53" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C53" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D53" s="2">
         <v>45326</v>
@@ -2572,7 +2572,7 @@
         <v>46446</v>
       </c>
       <c r="G53" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H53" t="str">
         <f>VLOOKUP($G53,Properties[],2,FALSE)</f>
@@ -2593,10 +2593,10 @@
     </row>
     <row r="54" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B54" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C54" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D54" s="2">
         <v>45333</v>
@@ -2608,7 +2608,7 @@
         <v>46446</v>
       </c>
       <c r="G54" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H54" t="str">
         <f>VLOOKUP($G54,Properties[],2,FALSE)</f>
@@ -2629,10 +2629,10 @@
     </row>
     <row r="55" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B55" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C55" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D55" s="2">
         <v>45399</v>
@@ -2644,7 +2644,7 @@
         <v>46507</v>
       </c>
       <c r="G55" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H55" t="str">
         <f>VLOOKUP($G55,Properties[],2,FALSE)</f>
@@ -2665,10 +2665,10 @@
     </row>
     <row r="56" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B56" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C56" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D56" s="2">
         <v>45499</v>
@@ -2680,7 +2680,7 @@
         <v>46599</v>
       </c>
       <c r="G56" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H56" t="str">
         <f>VLOOKUP($G56,Properties[],2,FALSE)</f>
@@ -2701,10 +2701,10 @@
     </row>
     <row r="57" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B57" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C57" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D57" s="2">
         <v>45474</v>
@@ -2716,7 +2716,7 @@
         <v>46599</v>
       </c>
       <c r="G57" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H57" t="str">
         <f>VLOOKUP($G57,Properties[],2,FALSE)</f>
@@ -2737,10 +2737,10 @@
     </row>
     <row r="58" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B58" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C58" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D58" s="2">
         <v>45445</v>
@@ -2752,7 +2752,7 @@
         <v>46568</v>
       </c>
       <c r="G58" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H58" t="str">
         <f>VLOOKUP($G58,Properties[],2,FALSE)</f>
@@ -2773,10 +2773,10 @@
     </row>
     <row r="59" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B59" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C59" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D59" s="2">
         <v>45379</v>
@@ -2788,7 +2788,7 @@
         <v>46477</v>
       </c>
       <c r="G59" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H59" t="str">
         <f>VLOOKUP($G59,Properties[],2,FALSE)</f>
@@ -2809,10 +2809,10 @@
     </row>
     <row r="60" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B60" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C60" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D60" s="2">
         <v>45445</v>
@@ -2824,7 +2824,7 @@
         <v>46568</v>
       </c>
       <c r="G60" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H60" t="str">
         <f>VLOOKUP($G60,Properties[],2,FALSE)</f>
@@ -2857,7 +2857,7 @@
   <dimension ref="B10:G60"/>
   <sheetViews>
     <sheetView topLeftCell="A2" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10:F10"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2887,12 +2887,12 @@
         <v>5</v>
       </c>
       <c r="G10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C11" t="s">
         <v>7</v>
@@ -2912,7 +2912,7 @@
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C12" t="s">
         <v>7</v>
@@ -2932,7 +2932,7 @@
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C13" t="s">
         <v>7</v>
@@ -2952,7 +2952,7 @@
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C14" t="s">
         <v>7</v>
@@ -2972,7 +2972,7 @@
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C15" t="s">
         <v>7</v>
@@ -2992,7 +2992,7 @@
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C16" t="s">
         <v>7</v>
@@ -3012,7 +3012,7 @@
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C17" t="s">
         <v>7</v>
@@ -3032,7 +3032,7 @@
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C18" t="s">
         <v>7</v>
@@ -3052,7 +3052,7 @@
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C19" t="s">
         <v>7</v>
@@ -3072,7 +3072,7 @@
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C20" t="s">
         <v>7</v>
@@ -3092,7 +3092,7 @@
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C21" t="s">
         <v>7</v>
@@ -3112,7 +3112,7 @@
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C22" t="s">
         <v>7</v>
@@ -3132,7 +3132,7 @@
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C23" t="s">
         <v>7</v>
@@ -3152,7 +3152,7 @@
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C24" t="s">
         <v>7</v>
@@ -3172,7 +3172,7 @@
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C25" t="s">
         <v>7</v>
@@ -3192,7 +3192,7 @@
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C26" t="s">
         <v>7</v>
@@ -3212,7 +3212,7 @@
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C27" t="s">
         <v>7</v>
@@ -3232,7 +3232,7 @@
     </row>
     <row r="28" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C28" t="s">
         <v>7</v>
@@ -3252,7 +3252,7 @@
     </row>
     <row r="29" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C29" t="s">
         <v>7</v>
@@ -3272,7 +3272,7 @@
     </row>
     <row r="30" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B30" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C30" t="s">
         <v>7</v>
@@ -3292,10 +3292,10 @@
     </row>
     <row r="31" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B31" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C31" t="s">
-        <v>8</v>
+        <v>169</v>
       </c>
       <c r="D31" t="str">
         <f>VLOOKUP($C31,PropertyType[],2,FALSE)</f>
@@ -3312,10 +3312,10 @@
     </row>
     <row r="32" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C32" t="s">
-        <v>8</v>
+        <v>169</v>
       </c>
       <c r="D32" t="str">
         <f>VLOOKUP($C32,PropertyType[],2,FALSE)</f>
@@ -3332,10 +3332,10 @@
     </row>
     <row r="33" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B33" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C33" t="s">
-        <v>8</v>
+        <v>169</v>
       </c>
       <c r="D33" t="str">
         <f>VLOOKUP($C33,PropertyType[],2,FALSE)</f>
@@ -3352,10 +3352,10 @@
     </row>
     <row r="34" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B34" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C34" t="s">
-        <v>8</v>
+        <v>169</v>
       </c>
       <c r="D34" t="str">
         <f>VLOOKUP($C34,PropertyType[],2,FALSE)</f>
@@ -3372,10 +3372,10 @@
     </row>
     <row r="35" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B35" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C35" t="s">
-        <v>8</v>
+        <v>169</v>
       </c>
       <c r="D35" t="str">
         <f>VLOOKUP($C35,PropertyType[],2,FALSE)</f>
@@ -3392,10 +3392,10 @@
     </row>
     <row r="36" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B36" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C36" t="s">
-        <v>8</v>
+        <v>169</v>
       </c>
       <c r="D36" t="str">
         <f>VLOOKUP($C36,PropertyType[],2,FALSE)</f>
@@ -3412,10 +3412,10 @@
     </row>
     <row r="37" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B37" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C37" t="s">
-        <v>8</v>
+        <v>169</v>
       </c>
       <c r="D37" t="str">
         <f>VLOOKUP($C37,PropertyType[],2,FALSE)</f>
@@ -3432,10 +3432,10 @@
     </row>
     <row r="38" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B38" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C38" t="s">
-        <v>8</v>
+        <v>169</v>
       </c>
       <c r="D38" t="str">
         <f>VLOOKUP($C38,PropertyType[],2,FALSE)</f>
@@ -3452,10 +3452,10 @@
     </row>
     <row r="39" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B39" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C39" t="s">
-        <v>8</v>
+        <v>169</v>
       </c>
       <c r="D39" t="str">
         <f>VLOOKUP($C39,PropertyType[],2,FALSE)</f>
@@ -3472,10 +3472,10 @@
     </row>
     <row r="40" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B40" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C40" t="s">
-        <v>8</v>
+        <v>169</v>
       </c>
       <c r="D40" t="str">
         <f>VLOOKUP($C40,PropertyType[],2,FALSE)</f>
@@ -3492,10 +3492,10 @@
     </row>
     <row r="41" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B41" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C41" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D41" t="str">
         <f>VLOOKUP($C41,PropertyType[],2,FALSE)</f>
@@ -3512,10 +3512,10 @@
     </row>
     <row r="42" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B42" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C42" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D42" t="str">
         <f>VLOOKUP($C42,PropertyType[],2,FALSE)</f>
@@ -3532,10 +3532,10 @@
     </row>
     <row r="43" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B43" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C43" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D43" t="str">
         <f>VLOOKUP($C43,PropertyType[],2,FALSE)</f>
@@ -3552,10 +3552,10 @@
     </row>
     <row r="44" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B44" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C44" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D44" t="str">
         <f>VLOOKUP($C44,PropertyType[],2,FALSE)</f>
@@ -3572,10 +3572,10 @@
     </row>
     <row r="45" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B45" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C45" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D45" t="str">
         <f>VLOOKUP($C45,PropertyType[],2,FALSE)</f>
@@ -3592,10 +3592,10 @@
     </row>
     <row r="46" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B46" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C46" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D46" t="str">
         <f>VLOOKUP($C46,PropertyType[],2,FALSE)</f>
@@ -3612,10 +3612,10 @@
     </row>
     <row r="47" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B47" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C47" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D47" t="str">
         <f>VLOOKUP($C47,PropertyType[],2,FALSE)</f>
@@ -3632,10 +3632,10 @@
     </row>
     <row r="48" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B48" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C48" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D48" t="str">
         <f>VLOOKUP($C48,PropertyType[],2,FALSE)</f>
@@ -3652,10 +3652,10 @@
     </row>
     <row r="49" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B49" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C49" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D49" t="str">
         <f>VLOOKUP($C49,PropertyType[],2,FALSE)</f>
@@ -3672,10 +3672,10 @@
     </row>
     <row r="50" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B50" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C50" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D50" t="str">
         <f>VLOOKUP($C50,PropertyType[],2,FALSE)</f>
@@ -3692,10 +3692,10 @@
     </row>
     <row r="51" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B51" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C51" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D51" t="str">
         <f>VLOOKUP($C51,PropertyType[],2,FALSE)</f>
@@ -3712,10 +3712,10 @@
     </row>
     <row r="52" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B52" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C52" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D52" t="str">
         <f>VLOOKUP($C52,PropertyType[],2,FALSE)</f>
@@ -3732,10 +3732,10 @@
     </row>
     <row r="53" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B53" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C53" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D53" t="str">
         <f>VLOOKUP($C53,PropertyType[],2,FALSE)</f>
@@ -3752,10 +3752,10 @@
     </row>
     <row r="54" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B54" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C54" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D54" t="str">
         <f>VLOOKUP($C54,PropertyType[],2,FALSE)</f>
@@ -3772,10 +3772,10 @@
     </row>
     <row r="55" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B55" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C55" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D55" t="str">
         <f>VLOOKUP($C55,PropertyType[],2,FALSE)</f>
@@ -3792,10 +3792,10 @@
     </row>
     <row r="56" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B56" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C56" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D56" t="str">
         <f>VLOOKUP($C56,PropertyType[],2,FALSE)</f>
@@ -3812,10 +3812,10 @@
     </row>
     <row r="57" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B57" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C57" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D57" t="str">
         <f>VLOOKUP($C57,PropertyType[],2,FALSE)</f>
@@ -3832,10 +3832,10 @@
     </row>
     <row r="58" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B58" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C58" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D58" t="str">
         <f>VLOOKUP($C58,PropertyType[],2,FALSE)</f>
@@ -3852,10 +3852,10 @@
     </row>
     <row r="59" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B59" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C59" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D59" t="str">
         <f>VLOOKUP($C59,PropertyType[],2,FALSE)</f>
@@ -3872,10 +3872,10 @@
     </row>
     <row r="60" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B60" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C60" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D60" t="str">
         <f>VLOOKUP($C60,PropertyType[],2,FALSE)</f>
@@ -3905,7 +3905,7 @@
   <dimension ref="B10:E13"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3935,7 +3935,7 @@
         <v>7</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D11" s="1">
         <v>5535</v>
@@ -3946,10 +3946,10 @@
     </row>
     <row r="12" spans="2:5" ht="80" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
-        <v>8</v>
+        <v>169</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D12" s="1">
         <v>4250</v>
@@ -3960,10 +3960,10 @@
     </row>
     <row r="13" spans="2:5" ht="160" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D13" s="1">
         <v>3125</v>

</xml_diff>